<commit_message>
TP A1 et A2-4-D du 24/01/2024
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francksilvestre/Documents/12_WS-Enseignement/BUT2/S4/R4-02-Qual-Developpement/R4-02-Qualite-Developpement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC64E15-3F2A-334A-927E-CFB988FBA576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F471088-D603-4BFE-B666-940410C90404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>La notice de démarrage a permis de fluidifier la partie config.</t>
+  </si>
+  <si>
+    <t>Simple stack =&gt; #2.1 en cours pour la plupart, terminé pour certains. A terminer pour la semaine prochaine.</t>
+  </si>
+  <si>
+    <t>Certains ont du mal à paramétrer le proxy malgré la notice. Peut-être modifier la notice avec Adresse de configuration automatique du proxy : http://cache.iut-rodez.fr/proxy.pac</t>
+  </si>
+  <si>
+    <t>Inégalité d'autonomie dans l'utilisation de la notice. L'application du override pour le paramétrage Maven a régulièrement été oublié…</t>
+  </si>
+  <si>
+    <t>Pour certains, il n'est pas clair que pour la #2.1 il faut implémenter le contenu de la classe SimpleStack avec sa structure de données interne, sans modifier les tests… Je me suis posé la même question lorsque j'ai fait le TP de mon côté, mais j'ai rapidement compris. Peut-être que ce doute nuit à certains. Par ailleurs, savoir qu'il faut utiliser une structure comme ArrayList en interne n'est pas automatique pour tous...</t>
+  </si>
+  <si>
+    <t>expliciter "encore plus" ce qui est demandé pour les quelques qui ont du mal à demarrer (coder la structure interne avec un ArrayList) et limiter la charge cognitive ?</t>
   </si>
 </sst>
 </file>
@@ -500,23 +515,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="13.375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="41.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
+    <col min="7" max="7" width="41.375" customWidth="1"/>
     <col min="8" max="8" width="46" customWidth="1"/>
     <col min="9" max="9" width="79.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,9 +560,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>45236</v>
+        <v>45314</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -574,9 +589,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45315</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
@@ -593,39 +612,59 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+    <row r="4" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45315</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>45237</v>
+        <v>45315</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>45243</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -634,7 +673,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -645,13 +684,9 @@
       <c r="H7" s="4"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>45244</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -660,13 +695,9 @@
       <c r="H8" s="4"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>45250</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -675,7 +706,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -686,13 +717,9 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>45251</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -701,13 +728,9 @@
       <c r="H11" s="4"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>45258</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -716,7 +739,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -727,13 +750,9 @@
       <c r="H13" s="4"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>45258</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -742,13 +761,9 @@
       <c r="H14" s="4"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>45264</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -757,13 +772,9 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>45265</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>12</v>
-      </c>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -772,7 +783,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -783,7 +794,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -794,7 +805,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -805,7 +816,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -816,7 +827,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -827,7 +838,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -838,7 +849,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -849,7 +860,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -860,7 +871,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -871,7 +882,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -882,7 +893,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -893,7 +904,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -904,7 +915,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -915,7 +926,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -926,7 +937,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>

</xml_diff>

<commit_message>
TPA2-A4-D et TPA3 du 30/01/2024
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90552BC-0442-4B37-B629-9639F2C0029D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="2023-2024"/>
+    <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -95,13 +101,33 @@
   </si>
   <si>
     <t>Il a fallu rappeler comment activer la licence et à l'arrivée sur QuestionScore la config Maven. Ce groupe est hyper hétérogène :-(. Difficile de trouver la cadence quand tout le monde doit être aligné (mode Kata)</t>
+  </si>
+  <si>
+    <t>Simple stack : correction #2.1 + indications de correction données pour finir jusqu'à #2.3.
+Finir #2.2 et #2.3 + préparer projet Questionsscore pour la prochaine fois.</t>
+  </si>
+  <si>
+    <t>Simple stack : correction #2.2 et #2.3.
+Debut questionsscore : #0 et debut kata sur #1. J'ai montré comment faire un Generate de Test.</t>
+  </si>
+  <si>
+    <t>Certains font un clone via Gitbash dans le même répertoir sans utiliser l'interface Get From VCS de IntelliJ et ça pose des problèmes… clarifier qu'il faut toujours passer par IntelliJ pour cloner le dépôt.</t>
+  </si>
+  <si>
+    <t>Certains oublient le testPeekOnEmptyStack. La démarche générale semble avoir été comprise.
+Il a fallu du temps à certains pour réactiver la licence sur le poste, avec la manipulation du proxy…</t>
+  </si>
+  <si>
+    <t>Pas de problème particulier. Le groupe a bien compris.
+Certains testent assertNotThrown dans un cas nominal de peek ou pop, mais ce n'est pas utile il me semble car si une exception est levée, le test ne passe pas.
+Ils ont des souvenirs de l'utilisation d'Eclipse dans lequel il faudrait faire ça pour que les tests passents sans se bloquer. 
+Or dans IntelliJ les tests semblent bien tous indépendants.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,67 +170,75 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I31" displayName="Tableau1" name="Tableau1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:I31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:I31" totalsRowShown="0">
+  <autoFilter ref="A1:I31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn name="Date" id="1"/>
-    <tableColumn name="Enseignant" id="2"/>
-    <tableColumn name="Séance" id="3"/>
-    <tableColumn name="Groupe A1" id="4"/>
-    <tableColumn name="Groupe A2-4" id="5"/>
-    <tableColumn name="Groupe A3" id="6"/>
-    <tableColumn name="Description" id="7"/>
-    <tableColumn name="Améliortions pour l'année prochaine" id="8"/>
-    <tableColumn name="Commentaires" id="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Enseignant"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Séance"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Groupe A1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Groupe A2-4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Groupe A3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Améliortions pour l'année prochaine"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Commentaires"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -213,10 +247,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -254,71 +288,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -346,7 +380,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -369,11 +403,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -382,13 +416,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -398,7 +432,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -407,7 +441,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -416,7 +450,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -424,10 +458,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -492,28 +526,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="8" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="41.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="46.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="79.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.54296875" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25" customFormat="1" s="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -542,7 +578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="28.5">
+    <row r="2" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>45314</v>
       </c>
@@ -571,7 +607,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="28.5">
+    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>45315</v>
       </c>
@@ -594,7 +630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="51">
+    <row r="4" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>45315</v>
       </c>
@@ -619,7 +655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="62.25">
+    <row r="5" spans="1:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>45315</v>
       </c>
@@ -644,7 +680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="48">
+    <row r="6" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>45321</v>
       </c>
@@ -667,29 +703,55 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="7" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="13">
+        <v>45321</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="13">
+        <v>45321</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -700,7 +762,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -711,7 +773,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -722,7 +784,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -733,7 +795,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -744,7 +806,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -755,7 +817,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -766,7 +828,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -777,7 +839,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -788,7 +850,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -799,7 +861,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -810,7 +872,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -821,7 +883,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -832,7 +894,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -843,7 +905,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -854,7 +916,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -865,7 +927,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -876,7 +938,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -887,7 +949,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -898,7 +960,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -909,7 +971,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -920,7 +982,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -931,7 +993,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>

</xml_diff>

<commit_message>
Mise à jour tableau de nbord (oubli CM)
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90552BC-0442-4B37-B629-9639F2C0029D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="2023-2024"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -92,6 +86,15 @@
   </si>
   <si>
     <t>Pour certains, il n'est pas clair que pour la #2.1 il faut implémenter le contenu de la classe SimpleStack avec sa structure de données interne, sans modifier les tests… Je me suis posé la même question lorsque j'ai fait le TP de mon côté, mais j'ai rapidement compris. Peut-être que ce doute nuit à certains. Par ailleurs, savoir qu'il faut utiliser une structure comme ArrayList en interne n'est pas automatique pour tous...</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Question rappel pyramide des tests. Fin couverture du code, intro JUNIT.</t>
+  </si>
+  <si>
+    <t>La question de rappel, c'est bien.</t>
   </si>
   <si>
     <t>X</t>
@@ -107,15 +110,15 @@
 Finir #2.2 et #2.3 + préparer projet Questionsscore pour la prochaine fois.</t>
   </si>
   <si>
+    <t>Certains oublient le testPeekOnEmptyStack. La démarche générale semble avoir été comprise.
+Il a fallu du temps à certains pour réactiver la licence sur le poste, avec la manipulation du proxy…</t>
+  </si>
+  <si>
     <t>Simple stack : correction #2.2 et #2.3.
 Debut questionsscore : #0 et debut kata sur #1. J'ai montré comment faire un Generate de Test.</t>
   </si>
   <si>
     <t>Certains font un clone via Gitbash dans le même répertoir sans utiliser l'interface Get From VCS de IntelliJ et ça pose des problèmes… clarifier qu'il faut toujours passer par IntelliJ pour cloner le dépôt.</t>
-  </si>
-  <si>
-    <t>Certains oublient le testPeekOnEmptyStack. La démarche générale semble avoir été comprise.
-Il a fallu du temps à certains pour réactiver la licence sur le poste, avec la manipulation du proxy…</t>
   </si>
   <si>
     <t>Pas de problème particulier. Le groupe a bien compris.
@@ -127,8 +130,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +143,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -170,75 +180,82 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="16">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:I31" totalsRowShown="0">
-  <autoFilter ref="A1:I31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I32" displayName="Tableau1" name="Tableau1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Enseignant"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Séance"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Groupe A1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Groupe A2-4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Groupe A3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Améliortions pour l'année prochaine"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Commentaires"/>
+    <tableColumn name="Date" id="1"/>
+    <tableColumn name="Enseignant" id="2"/>
+    <tableColumn name="Séance" id="3"/>
+    <tableColumn name="Groupe A1" id="4"/>
+    <tableColumn name="Groupe A2-4" id="5"/>
+    <tableColumn name="Groupe A3" id="6"/>
+    <tableColumn name="Description" id="7"/>
+    <tableColumn name="Améliortions pour l'année prochaine" id="8"/>
+    <tableColumn name="Commentaires" id="9"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -247,10 +264,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -288,71 +305,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -380,7 +397,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -403,11 +420,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -416,13 +433,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -432,7 +449,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -441,7 +458,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -450,7 +467,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -458,10 +475,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -526,30 +543,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="79.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="13" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="41.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="15" width="46.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="14" width="79.57642857142856" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -578,7 +593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33">
       <c r="A2" s="5">
         <v>45314</v>
       </c>
@@ -607,7 +622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33">
       <c r="A3" s="5">
         <v>45315</v>
       </c>
@@ -630,7 +645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60.75">
       <c r="A4" s="5">
         <v>45315</v>
       </c>
@@ -655,7 +670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="74.25">
       <c r="A5" s="5">
         <v>45315</v>
       </c>
@@ -680,54 +695,58 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="7">
+        <v>45320</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25">
+      <c r="A7" s="5">
         <v>45321</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="13">
-        <v>45321</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12" t="s">
+      <c r="D7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="87" x14ac:dyDescent="0.35">
-      <c r="A8" s="13">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="51">
+      <c r="A8" s="10">
         <v>45321</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -737,32 +756,44 @@
         <v>15</v>
       </c>
       <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="88.5">
+      <c r="A9" s="10">
+        <v>45321</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -773,7 +804,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -782,9 +813,9 @@
       <c r="F11" s="6"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -795,7 +826,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -806,7 +837,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -817,7 +848,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -826,9 +857,9 @@
       <c r="F15" s="6"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -839,7 +870,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -848,9 +879,9 @@
       <c r="F17" s="6"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -861,7 +892,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -870,9 +901,9 @@
       <c r="F19" s="6"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I19" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -883,7 +914,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -894,7 +925,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -905,7 +936,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -914,10 +945,10 @@
       <c r="F23" s="6"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+      <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -927,8 +958,8 @@
       <c r="H24" s="4"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+      <c r="A25" s="12"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -938,7 +969,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -949,7 +980,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -960,7 +991,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -971,7 +1002,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -982,7 +1013,7 @@
       <c r="H29" s="4"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -993,7 +1024,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1004,6 +1035,17 @@
       <c r="H31" s="4"/>
       <c r="I31" s="6"/>
     </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
CM et TP A1  des 5 et 6 février 2024
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -125,6 +125,18 @@
 Certains testent assertNotThrown dans un cas nominal de peek ou pop, mais ce n'est pas utile il me semble car si une exception est levée, le test ne passe pas.
 Ils ont des souvenirs de l'utilisation d'Eclipse dans lequel il faudrait faire ça pour que les tests passents sans se bloquer. 
 Or dans IntelliJ les tests semblent bien tous indépendants.</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Rappel, pyramide des tests. Fin cours (mock). Questions elaastic sur TDD.</t>
+  </si>
+  <si>
+    <t>Cours de fin journée : les étudiants et moi fatigués ; ambiance de travail médiocre. C'est rare avec ce groupe pour le signaler.</t>
+  </si>
+  <si>
+    <t>Fix #2 de question score. RAS.</t>
   </si>
 </sst>
 </file>
@@ -142,13 +154,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -180,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,31 +203,22 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -553,15 +556,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="41.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="15" width="46.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="14" width="79.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="41.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="46.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="79.57642857142856" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
@@ -583,10 +586,10 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -594,172 +597,172 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>45314</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>45315</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60.75">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>45315</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="4" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="74.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>45315</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="4" t="s">
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="7">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="28.5">
+      <c r="A6" s="6">
         <v>45320</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="9" t="s">
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="8" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>45321</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="51">
-      <c r="A8" s="10">
+      <c r="A8" s="4">
         <v>45321</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="11"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="3" t="s">
         <v>30</v>
       </c>
@@ -769,282 +772,308 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="88.5">
-      <c r="A9" s="10">
+      <c r="A9" s="4">
         <v>45321</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="A10" s="4">
+        <v>45327</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="A11" s="4">
+        <v>45328</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="6"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="6"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="6"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="6"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="6"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="6"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="6"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="6"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="6"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
JDB TPA3 du 06/02/2024
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0611AC5-CBEB-48E0-B715-4431E18E6A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="2023-2024"/>
+    <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -127,9 +133,6 @@
 Or dans IntelliJ les tests semblent bien tous indépendants.</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>Rappel, pyramide des tests. Fin cours (mock). Questions elaastic sur TDD.</t>
   </si>
   <si>
@@ -137,13 +140,18 @@
   </si>
   <si>
     <t>Fix #2 de question score. RAS.</t>
+  </si>
+  <si>
+    <t>QuestionsScore Fix #1 en kata</t>
+  </si>
+  <si>
+    <t>On a avancé jusqu'à écrire des cas nominaux et cas limites pour le constructeur de QCE (énoncé vide ou null, indice &lt; 1), et du score pour indice &lt; 1. Factorisation avec BeforeEach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,72 +201,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I32" displayName="Tableau1" name="Tableau1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:I32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:I32" totalsRowShown="0">
+  <autoFilter ref="A1:I32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn name="Date" id="1"/>
-    <tableColumn name="Enseignant" id="2"/>
-    <tableColumn name="Séance" id="3"/>
-    <tableColumn name="Groupe A1" id="4"/>
-    <tableColumn name="Groupe A2-4" id="5"/>
-    <tableColumn name="Groupe A3" id="6"/>
-    <tableColumn name="Description" id="7"/>
-    <tableColumn name="Améliortions pour l'année prochaine" id="8"/>
-    <tableColumn name="Commentaires" id="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Enseignant"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Séance"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Groupe A1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Groupe A2-4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Groupe A3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Améliortions pour l'année prochaine"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Commentaires"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -267,10 +278,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -308,71 +319,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,7 +411,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -423,11 +434,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -436,13 +447,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -452,7 +463,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -461,7 +472,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -470,7 +481,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -478,10 +489,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -546,28 +557,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="10" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="41.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="46.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="79.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="15" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.54296875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -596,7 +609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33">
+    <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45314</v>
       </c>
@@ -625,7 +638,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33">
+    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>45315</v>
       </c>
@@ -648,7 +661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60.75">
+    <row r="4" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>45315</v>
       </c>
@@ -673,7 +686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="74.25">
+    <row r="5" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>45315</v>
       </c>
@@ -698,7 +711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="28.5">
+    <row r="6" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>45320</v>
       </c>
@@ -725,7 +738,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25">
+    <row r="7" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>45321</v>
       </c>
@@ -748,7 +761,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="51">
+    <row r="8" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>45321</v>
       </c>
@@ -771,7 +784,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="88.5">
+    <row r="9" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>45321</v>
       </c>
@@ -796,7 +809,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>45327</v>
       </c>
@@ -804,26 +817,26 @@
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>45328</v>
       </c>
@@ -839,23 +852,35 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>45328</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="I12" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -866,7 +891,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -877,7 +902,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -888,7 +913,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -899,7 +924,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -910,7 +935,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -921,7 +946,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -932,7 +957,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -943,7 +968,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -954,7 +979,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -965,7 +990,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -976,7 +1001,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -987,7 +1012,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -998,7 +1023,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1009,7 +1034,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1020,7 +1045,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1031,7 +1056,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1042,7 +1067,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1053,7 +1078,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1064,7 +1089,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>

</xml_diff>

<commit_message>
TP A3 du 13/02/2024
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A47AB0F-CEAD-45CF-B973-921EFB35A71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="2023-2024"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -150,12 +144,20 @@
   <si>
     <t>Idem TPA3. Par contre le lecteur Z a planté en fin de séance, ce qui a compliqué les choses.</t>
   </si>
+  <si>
+    <t>QuestionsScore fix #2 : ce qui n'ont pas fini doivent finir pour la prochaine séance afin que tout le monde démarre la question 3</t>
+  </si>
+  <si>
+    <t>Groupe très hétérogène.
+&lt;!&gt; Problème de licence serveur Intellij. Le SI est sur le coup mais cela ne fonctionne pas, il fut donc que les étudiants laisse le proxy activé, et choisisse un licence associée à un compte jetbrins qu'ils crééent si ils ne l'ont pas déjà avec l'adresse en ut-capitole pour avoir leur propre licence education...</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,12 +168,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -203,76 +199,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="10">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:I32" totalsRowShown="0">
-  <autoFilter ref="A1:I32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I32" displayName="Tableau1" name="Tableau1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Enseignant"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Séance"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Groupe A1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Groupe A2-4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Groupe A3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Améliortions pour l'année prochaine"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Commentaires"/>
+    <tableColumn name="Date" id="1"/>
+    <tableColumn name="Enseignant" id="2"/>
+    <tableColumn name="Séance" id="3"/>
+    <tableColumn name="Groupe A1" id="4"/>
+    <tableColumn name="Groupe A2-4" id="5"/>
+    <tableColumn name="Groupe A3" id="6"/>
+    <tableColumn name="Description" id="7"/>
+    <tableColumn name="Améliortions pour l'année prochaine" id="8"/>
+    <tableColumn name="Commentaires" id="9"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -281,10 +265,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -322,71 +306,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -414,7 +398,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -437,11 +421,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -450,13 +434,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -466,7 +450,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -475,7 +459,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -484,7 +468,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -492,10 +476,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -560,30 +544,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G8" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="79.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="7" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="41.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="46.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="79.57642857142856" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -612,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33">
       <c r="A2" s="4">
         <v>45314</v>
       </c>
@@ -641,7 +623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33">
       <c r="A3" s="4">
         <v>45315</v>
       </c>
@@ -664,7 +646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60.75">
       <c r="A4" s="4">
         <v>45315</v>
       </c>
@@ -689,7 +671,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="74.25">
       <c r="A5" s="4">
         <v>45315</v>
       </c>
@@ -714,34 +696,34 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="28.5">
+      <c r="A6" s="4">
         <v>45320</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="7" t="s">
+      <c r="H6" s="3"/>
+      <c r="I6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25">
       <c r="A7" s="4">
         <v>45321</v>
       </c>
@@ -764,7 +746,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="60.75">
       <c r="A8" s="4">
         <v>45321</v>
       </c>
@@ -787,7 +769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="88.5">
       <c r="A9" s="4">
         <v>45321</v>
       </c>
@@ -812,7 +794,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33">
       <c r="A10" s="4">
         <v>45327</v>
       </c>
@@ -839,7 +821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>45328</v>
       </c>
@@ -860,7 +842,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>45328</v>
       </c>
@@ -883,7 +865,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>45330</v>
       </c>
@@ -906,18 +888,30 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="51.75">
+      <c r="A14" s="4">
+        <v>45335</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="3"/>
+      <c r="F14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -928,7 +922,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -939,7 +933,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -950,7 +944,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -961,7 +955,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -972,7 +966,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -983,7 +977,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -994,7 +988,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1005,7 +999,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1016,7 +1010,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1027,8 +1021,8 @@
       <c r="H24" s="3"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+      <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -1038,7 +1032,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1049,7 +1043,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1060,7 +1054,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1071,7 +1065,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1082,7 +1076,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1093,7 +1087,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1104,7 +1098,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>

</xml_diff>

<commit_message>
CR TPs du 15/02
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7730D809-CA41-42A0-8318-1A12F9C97C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -164,17 +158,21 @@
     <t>Travail sur QuestionsScore fix #3.</t>
   </si>
   <si>
-    <t>Certains ont eu des difficultés lors du test du constructeur avec enonce vide ou null. Selon l'ordre des verification null et isEmpty, et les deux assertThrows dans le même test, un des deux peut ne pas passer… (null est considéré comme vide…)</t>
-  </si>
-  <si>
     <t>Ce groupe dit qu'ils avaient reçu pour consigne de ne pas toucher à la classe principale, donc pas de qualité des tests en rajoutant les cas limites évoqués avec les deux autres groupes. Du coup, pas de modif de la classe pour la question #4.</t>
+  </si>
+  <si>
+    <t>Règle métier du #4 à expliciter sur les points négatifs pour réponses erronées.</t>
+  </si>
+  <si>
+    <t>Certains ont eu des difficultés lors du test du constructeur avec enonce vide ou null. Selon l'ordre des verification null et isEmpty, et les deux assertThrows dans le même test, un des deux peut ne pas passer… (null est considéré comme vide…).
+Problème avec Mattéo Faussurier pour Run sa classe de tests... Présence dans le pom.xml d'une dépendance RELEASE au niveau de JUnit... ?!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,18 +261,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:I32" totalsRowShown="0">
-  <autoFilter ref="A1:I32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:I32" totalsRowShown="0">
+  <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Enseignant"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Séance"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Groupe A1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Groupe A2-4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Groupe A3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Améliortions pour l'année prochaine"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Commentaires"/>
+    <tableColumn id="1" name="Date"/>
+    <tableColumn id="2" name="Enseignant"/>
+    <tableColumn id="3" name="Séance"/>
+    <tableColumn id="4" name="Groupe A1"/>
+    <tableColumn id="5" name="Groupe A2-4"/>
+    <tableColumn id="6" name="Groupe A3"/>
+    <tableColumn id="7" name="Description"/>
+    <tableColumn id="8" name="Améliortions pour l'année prochaine"/>
+    <tableColumn id="9" name="Commentaires"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -564,30 +562,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="79.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.5703125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -616,7 +614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="33" customHeight="1">
       <c r="A2" s="4">
         <v>45314</v>
       </c>
@@ -645,7 +643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="33" customHeight="1">
       <c r="A3" s="4">
         <v>45315</v>
       </c>
@@ -668,7 +666,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="60.75" customHeight="1">
       <c r="A4" s="4">
         <v>45315</v>
       </c>
@@ -693,7 +691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="74.25" customHeight="1">
       <c r="A5" s="4">
         <v>45315</v>
       </c>
@@ -718,7 +716,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="28.5" customHeight="1">
       <c r="A6" s="4">
         <v>45320</v>
       </c>
@@ -745,7 +743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="47.25" customHeight="1">
       <c r="A7" s="4">
         <v>45321</v>
       </c>
@@ -768,7 +766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="60.75" customHeight="1">
       <c r="A8" s="4">
         <v>45321</v>
       </c>
@@ -791,7 +789,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="88.5" customHeight="1">
       <c r="A9" s="4">
         <v>45321</v>
       </c>
@@ -816,7 +814,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="33" customHeight="1">
       <c r="A10" s="4">
         <v>45327</v>
       </c>
@@ -843,7 +841,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1">
       <c r="A11" s="4">
         <v>45328</v>
       </c>
@@ -864,7 +862,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1">
       <c r="A12" s="4">
         <v>45328</v>
       </c>
@@ -887,7 +885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="19.5" customHeight="1">
       <c r="A13" s="4">
         <v>45330</v>
       </c>
@@ -910,7 +908,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="51.75" customHeight="1">
       <c r="A14" s="4">
         <v>45335</v>
       </c>
@@ -933,7 +931,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="75">
       <c r="A15" s="4">
         <v>45337</v>
       </c>
@@ -952,11 +950,11 @@
         <v>43</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I15" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45">
       <c r="A16" s="4">
         <v>45337</v>
       </c>
@@ -974,12 +972,14 @@
       <c r="G16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="I16" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="19.5" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -990,7 +990,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="19.5" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1001,7 +1001,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="19.5" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1012,7 +1012,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="19.5" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1023,7 +1023,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="19.5" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1034,7 +1034,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="17.25" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1045,7 +1045,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1056,7 +1056,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1067,7 +1067,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1078,7 +1078,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1089,7 +1089,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1100,7 +1100,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1111,7 +1111,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1122,7 +1122,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1133,7 +1133,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1144,7 +1144,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>

</xml_diff>

<commit_message>
TP A3 du 27/02/2024 (yasmf hello_world)
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97661C3-9890-4F89-9915-7325AE6A1290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="2023-2024"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -142,6 +136,9 @@
     <t>Fix #2 de question score. RAS.</t>
   </si>
   <si>
+    <t>QuestionsScore fix #1 en kata</t>
+  </si>
+  <si>
     <t>On a avancé jusqu'à écrire des cas nominaux et cas limites pour le constructeur de QCE (énoncé vide ou null, indice &lt; 1), et du score pour indice &lt; 1. Factorisation avec BeforeEach</t>
   </si>
   <si>
@@ -155,36 +152,43 @@
 &lt;!&gt; Problème de licence serveur Intellij. Le SI est sur le coup mais cela ne fonctionne pas, il fut donc que les étudiants laisse le proxy activé, et choisisse un licence associée à un compte jetbrins qu'ils crééent si ils ne l'ont pas déjà avec l'adresse en ut-capitole pour avoir leur propre licence education...</t>
   </si>
   <si>
-    <t>QuestionsScore fix #1 en kata</t>
-  </si>
-  <si>
     <t>Travail sur QuestionsScore fix #2.</t>
-  </si>
-  <si>
-    <t>Travail sur QuestionsScore fix #3.</t>
-  </si>
-  <si>
-    <t>Ce groupe dit qu'ils avaient reçu pour consigne de ne pas toucher à la classe principale, donc pas de qualité des tests en rajoutant les cas limites évoqués avec les deux autres groupes. Du coup, pas de modif de la classe pour la question #4.</t>
-  </si>
-  <si>
-    <t>Règle métier du #4 à expliciter sur les points négatifs pour réponses erronées.</t>
   </si>
   <si>
     <t>Certains ont eu des difficultés lors du test du constructeur avec enonce vide ou null. Selon l'ordre des verification null et isEmpty, et les deux assertThrows dans le même test, un des deux peut ne pas passer… (null est considéré comme vide…).
 Problème avec Mattéo Faussurier pour Run sa classe de tests... Présence dans le pom.xml d'une dépendance RELEASE au niveau de JUnit... ?!</t>
   </si>
   <si>
+    <t>Travail sur QuestionsScore fix #3.</t>
+  </si>
+  <si>
+    <t>Règle métier du #4 à expliciter sur les points négatifs pour réponses erronées.</t>
+  </si>
+  <si>
+    <t>Ce groupe dit qu'ils avaient reçu pour consigne de ne pas toucher à la classe principale, donc pas de qualité des tests en rajoutant les cas limites évoqués avec les deux autres groupes. Du coup, pas de modif de la classe pour la question #4.</t>
+  </si>
+  <si>
     <t>Commentaires retour sur évaluation.
 Elaastic Yasmf 1.6 : 1 à 4 (Hello World) fait et corrigé. 5 commencé, non corrigé (All Users)</t>
   </si>
   <si>
     <t>Il a fallu rappeler que Docker nécessite un clonage du dépôt en local (sur D) et pas sur Z. Peu sont allé voir en détail pour remonter la "piste" de autoload.php. Heureusement que Leila et Loic sont là.</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP sur exemples résolus yasmf =&gt; fin travail et questions sur Hello_world.RAF : travail et questions sur all_users. </t>
+  </si>
+  <si>
+    <t>Sur autoload, 8 réponses, et une restitution des résultats sans passer la phase 2.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,66 +232,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:I32" totalsRowShown="0">
-  <autoFilter ref="A1:I32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I32" displayName="Tableau1" name="Tableau1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Enseignant"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Séance"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Groupe A1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Groupe A2-4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Groupe A3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Améliortions pour l'année prochaine"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Commentaires"/>
+    <tableColumn name="Date" id="1"/>
+    <tableColumn name="Enseignant" id="2"/>
+    <tableColumn name="Séance" id="3"/>
+    <tableColumn name="Groupe A1" id="4"/>
+    <tableColumn name="Groupe A2-4" id="5"/>
+    <tableColumn name="Groupe A3" id="6"/>
+    <tableColumn name="Description" id="7"/>
+    <tableColumn name="Améliortions pour l'année prochaine" id="8"/>
+    <tableColumn name="Commentaires" id="9"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -296,10 +297,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -337,71 +338,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -429,7 +430,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -452,11 +453,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -465,13 +466,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -481,7 +482,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -490,7 +491,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -499,7 +500,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -507,10 +508,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -575,30 +576,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="79.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="7" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="41.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="46.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="79.57642857142856" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -627,7 +626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33">
       <c r="A2" s="4">
         <v>45314</v>
       </c>
@@ -656,7 +655,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33">
       <c r="A3" s="4">
         <v>45315</v>
       </c>
@@ -679,7 +678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60.75">
       <c r="A4" s="4">
         <v>45315</v>
       </c>
@@ -704,7 +703,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="74.25">
       <c r="A5" s="4">
         <v>45315</v>
       </c>
@@ -729,7 +728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33">
       <c r="A6" s="4">
         <v>45320</v>
       </c>
@@ -756,7 +755,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25">
       <c r="A7" s="4">
         <v>45321</v>
       </c>
@@ -779,7 +778,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="60.75">
       <c r="A8" s="4">
         <v>45321</v>
       </c>
@@ -802,7 +801,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="88.5">
       <c r="A9" s="4">
         <v>45321</v>
       </c>
@@ -827,7 +826,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33">
       <c r="A10" s="4">
         <v>45327</v>
       </c>
@@ -854,7 +853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>45328</v>
       </c>
@@ -875,7 +874,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>45328</v>
       </c>
@@ -891,14 +890,14 @@
         <v>11</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>45330</v>
       </c>
@@ -914,14 +913,14 @@
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="51.75">
       <c r="A14" s="4">
         <v>45335</v>
       </c>
@@ -937,14 +936,14 @@
         <v>11</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="4">
         <v>45337</v>
       </c>
@@ -964,10 +963,10 @@
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="4">
         <v>45337</v>
       </c>
@@ -983,16 +982,16 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>46</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="50.25">
       <c r="A17" s="4">
         <v>45349</v>
       </c>
@@ -1015,18 +1014,30 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="47.25">
+      <c r="A18" s="4">
+        <v>45349</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1037,7 +1048,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1048,7 +1059,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1059,7 +1070,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1070,7 +1081,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1081,7 +1092,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1092,7 +1103,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1103,7 +1114,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1114,7 +1125,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1125,7 +1136,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1136,7 +1147,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1147,7 +1158,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1158,7 +1169,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1169,7 +1180,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>

</xml_diff>

<commit_message>
TP A2-4-D du 4 mars 2024
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francksilvestre/Documents/12_WS-Enseignement/BUT2/S4/R4-02-Qual-Developpement/R4-02-Qualite-Developpement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CECE80D-86F0-4248-946F-F4C069332B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4E49D6-C63A-7746-8D89-2886D71553FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24480" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -201,6 +201,14 @@
   <si>
     <t>Suite et fin Elaastic Yasmf 1.6 : All Users (5, 6, 7 + PHPStan et tests PHPUnit sans et avec Coverage lancés).
 Suite de QuestionScore : fix #3 en cours de travail pour la majorité d'entre eux.</t>
+  </si>
+  <si>
+    <t>Suite et fin Elaastic Yasmf 1.6 : All Users (5, 6, 7 + PHPStan et tests PHPUnit sans et avec Coverage lancés).</t>
+  </si>
+  <si>
+    <t>J'ai insisté sur le fait que l'approche transaction+rollback était indispensable sur les tests d'intégration modififant une BD =&gt; à appliquer en SAÉ.
+On a pas eu le temps de rebasculer sur question score.
+Question : est-ce qu'ils utilisent bien les commits "fix #..." ? J'ai jeté un coup d'oeil au board Git4school et ai vu qu'un seul commit de fix #2...</t>
   </si>
 </sst>
 </file>
@@ -603,24 +611,24 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.5" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="79.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.5" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -649,7 +657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>45314</v>
       </c>
@@ -678,7 +686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>45315</v>
       </c>
@@ -701,7 +709,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>45315</v>
       </c>
@@ -726,7 +734,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>45315</v>
       </c>
@@ -751,7 +759,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>45320</v>
       </c>
@@ -778,7 +786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>45321</v>
       </c>
@@ -801,7 +809,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>45321</v>
       </c>
@@ -824,7 +832,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>45321</v>
       </c>
@@ -849,7 +857,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>45327</v>
       </c>
@@ -876,7 +884,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>45328</v>
       </c>
@@ -897,7 +905,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>45328</v>
       </c>
@@ -920,7 +928,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>45330</v>
       </c>
@@ -943,7 +951,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>45335</v>
       </c>
@@ -966,7 +974,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>45337</v>
       </c>
@@ -989,7 +997,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>45337</v>
       </c>
@@ -1014,7 +1022,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>45349</v>
       </c>
@@ -1037,7 +1045,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>45349</v>
       </c>
@@ -1060,7 +1068,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>45349</v>
       </c>
@@ -1085,7 +1093,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>45355</v>
       </c>
@@ -1108,18 +1116,30 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+    <row r="21" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>45355</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I21" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1130,7 +1150,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1141,7 +1161,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1152,7 +1172,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1163,7 +1183,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1174,7 +1194,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1185,7 +1205,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1196,7 +1216,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1207,7 +1227,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1218,7 +1238,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1229,7 +1249,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>

</xml_diff>

<commit_message>
TP A2_A4_D du 11 mars 2024
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D5DA0C-8785-4DF4-B39D-4DABC892AE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="2023-2024"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -178,22 +172,26 @@
 Elaastic Yasmf 1.6 : 1 à 4 (Hello World) fait et corrigé. 5 commencé, non corrigé (All Users)</t>
   </si>
   <si>
+    <t>Il a fallu rappeler que Docker nécessite un clonage du dépôt en local (sur D) et pas sur Z. Peu sont allé voir en détail pour remonter la "piste" de autoload.php. Heureusement que Leila et Loic sont là. Elaastic sans phase 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">TP sur exemples résolus yasmf =&gt; fin travail et questions sur Hello_world.RAF : travail et questions sur all_users. </t>
   </si>
   <si>
     <t>Sur autoload, 8 réponses, et une restitution des résultats sans passer la phase 2.</t>
   </si>
   <si>
+    <t>Elaastic Yasmf 1.6 : 1 à 4 (Hello World) fait et corrigé. 5 commencé, corrigé (All Users)</t>
+  </si>
+  <si>
     <t>La question 2 "Comment est récupéré YASMF dans l'application?" porte à confusion. Les étudiants ne savent pas si il s'agit des use/namespace, ou de l'appel de yamsf par composer.</t>
   </si>
   <si>
     <t>Elaastic sans phase 2</t>
   </si>
   <si>
-    <t>Il a fallu rappeler que Docker nécessite un clonage du dépôt en local (sur D) et pas sur Z. Peu sont allé voir en détail pour remonter la "piste" de autoload.php. Heureusement que Leila et Loic sont là. Elaastic sans phase 2</t>
-  </si>
-  <si>
-    <t>Elaastic Yasmf 1.6 : 1 à 4 (Hello World) fait et corrigé. 5 commencé, corrigé (All Users)</t>
+    <t>Suite et fin Elaastic Yasmf 1.6 : All Users (5, 6, 7 + PHPStan et tests PHPUnit sans et avec Coverage lancés) sans Phase 2
+Suite de QuestionScore : fix #3 en cours de travail pour la majorité d'entre eux.</t>
   </si>
   <si>
     <t>Ils ont pour la pluspart des difficultés a exprimer la différence entre un test unitaire et un test d'intégration. Les réponses à la question 5 sont globalement insuffisantes. Correction orale donnée.</t>
@@ -207,26 +205,26 @@
 Question : est-ce qu'ils utilisent bien les commits "fix #..." ? J'ai jeté un coup d'oeil au board Git4school et ai vu qu'un seul commit de fix #2...</t>
   </si>
   <si>
-    <t>Suite et fin Elaastic Yasmf 1.6 : All Users (5, 6, 7 + PHPStan et tests PHPUnit sans et avec Coverage lancés) sans Phase 2
-Suite de QuestionScore : fix #3 en cours de travail pour la majorité d'entre eux.</t>
-  </si>
-  <si>
     <t>Suite et fin Elaastic Yasmf 1.6 : All Users (5, 6, 7 + PHPStan et tests PHPUnit sans et avec Coverage lancés) avec Phase 2</t>
   </si>
   <si>
+    <t>Suite et fin QuestionScore (sauf pour certains), correction individuelle de chacun en passant les voir. Début ScrabbleScore.</t>
+  </si>
+  <si>
     <t>Ceux qui n'ont pas fini QuestionsScore doivent finir le #4, et accepter l'assignement ScrabbleScore pour la prochaine fois.</t>
   </si>
   <si>
-    <t>Suite et fin QuestionScore (sauf pour certains), correction individuelle de chacun en passant les voir. Début ScrabbleScore.</t>
-  </si>
-  <si>
     <t>idem. Problème spécial avec Fabien Serres… Maven fait des siennes on dirait…</t>
+  </si>
+  <si>
+    <t>Suite questionScore : fix #2, fix #3. RAF : correction application.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,66 +268,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:I32" totalsRowShown="0">
-  <autoFilter ref="A1:I32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I32" displayName="Tableau1" name="Tableau1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Enseignant"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Séance"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Groupe A1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Groupe A2-4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Groupe A3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Améliortions pour l'année prochaine"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Commentaires"/>
+    <tableColumn name="Date" id="1"/>
+    <tableColumn name="Enseignant" id="2"/>
+    <tableColumn name="Séance" id="3"/>
+    <tableColumn name="Groupe A1" id="4"/>
+    <tableColumn name="Groupe A2-4" id="5"/>
+    <tableColumn name="Groupe A3" id="6"/>
+    <tableColumn name="Description" id="7"/>
+    <tableColumn name="Améliortions pour l'année prochaine" id="8"/>
+    <tableColumn name="Commentaires" id="9"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
 </file>
 
@@ -338,10 +333,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -379,71 +374,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -471,7 +466,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -494,11 +489,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -507,13 +502,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -523,7 +518,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -532,7 +527,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -541,7 +536,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -549,10 +544,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -617,30 +612,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G20" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="79.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="7" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="41.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="46.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="79.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -669,7 +662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33">
       <c r="A2" s="4">
         <v>45314</v>
       </c>
@@ -698,7 +691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33">
       <c r="A3" s="4">
         <v>45315</v>
       </c>
@@ -721,7 +714,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60.75">
       <c r="A4" s="4">
         <v>45315</v>
       </c>
@@ -746,7 +739,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="74.25">
       <c r="A5" s="4">
         <v>45315</v>
       </c>
@@ -771,7 +764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33">
       <c r="A6" s="4">
         <v>45320</v>
       </c>
@@ -798,7 +791,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25">
       <c r="A7" s="4">
         <v>45321</v>
       </c>
@@ -821,7 +814,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="60.75">
       <c r="A8" s="4">
         <v>45321</v>
       </c>
@@ -844,7 +837,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="88.5">
       <c r="A9" s="4">
         <v>45321</v>
       </c>
@@ -869,7 +862,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33">
       <c r="A10" s="4">
         <v>45327</v>
       </c>
@@ -896,7 +889,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>45328</v>
       </c>
@@ -917,7 +910,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>45328</v>
       </c>
@@ -940,7 +933,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>45330</v>
       </c>
@@ -963,7 +956,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="51.75">
       <c r="A14" s="4">
         <v>45335</v>
       </c>
@@ -986,7 +979,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="4">
         <v>45337</v>
       </c>
@@ -1009,7 +1002,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="4">
         <v>45337</v>
       </c>
@@ -1034,7 +1027,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="50.25">
       <c r="A17" s="4">
         <v>45349</v>
       </c>
@@ -1054,10 +1047,10 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="47.25">
       <c r="A18" s="4">
         <v>45349</v>
       </c>
@@ -1073,14 +1066,14 @@
         <v>11</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="4">
         <v>45349</v>
       </c>
@@ -1096,16 +1089,16 @@
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="74.25">
       <c r="A20" s="4">
         <v>45355</v>
       </c>
@@ -1121,14 +1114,14 @@
         <v>11</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="74.25">
       <c r="A21" s="4">
         <v>45355</v>
       </c>
@@ -1144,14 +1137,14 @@
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="47.25">
       <c r="A22" s="4">
         <v>45356</v>
       </c>
@@ -1172,7 +1165,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="47.25">
       <c r="A23" s="4">
         <v>45362</v>
       </c>
@@ -1188,14 +1181,14 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="47.25">
       <c r="A24" s="4">
         <v>45362</v>
       </c>
@@ -1211,25 +1204,35 @@
         <v>11</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="39.75">
+      <c r="A25" s="6">
+        <v>45362</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="F25" s="5"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="H25" s="3"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1240,7 +1243,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1251,7 +1254,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1262,7 +1265,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1273,7 +1276,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1284,7 +1287,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1295,7 +1298,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>

</xml_diff>

<commit_message>
TP du 18 mars 2024 FSIL
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Suite questionScore : fix #2, fix #3. RAF : correction application.</t>
+  </si>
+  <si>
+    <t>18/03/2024</t>
+  </si>
+  <si>
+    <t>Fin question score pour tous (fix#4). 4 ont commencé en autonomie scrabble score.</t>
   </si>
 </sst>
 </file>
@@ -272,7 +278,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -287,7 +293,7 @@
     <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1233,13 +1239,23 @@
       <c r="I25" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="A26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="H26" s="3"/>
       <c r="I26" s="5"/>
     </row>

</xml_diff>

<commit_message>
TPA1 et A3 du 19/03/2024
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu.palosse\Documents\WorkspaceGit\BUT2\BUT2-R4-02-QualiteDeveloppement-Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC24053-FD1E-42F8-96EA-A45CC7B5C560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="2023-2024"/>
+    <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -225,12 +231,17 @@
   <si>
     <t>Fin question score pour tous (fix#4). 4 ont commencé en autonomie scrabble score.</t>
   </si>
+  <si>
+    <t>ScrabbleScore</t>
+  </si>
+  <si>
+    <t>présentation de la stratégie TDD à employer, puis travail en autonomie</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -274,63 +285,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I32" displayName="Tableau1" name="Tableau1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:I32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:I32" totalsRowShown="0">
+  <autoFilter ref="A1:I32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn name="Date" id="1"/>
-    <tableColumn name="Enseignant" id="2"/>
-    <tableColumn name="Séance" id="3"/>
-    <tableColumn name="Groupe A1" id="4"/>
-    <tableColumn name="Groupe A2-4" id="5"/>
-    <tableColumn name="Groupe A3" id="6"/>
-    <tableColumn name="Description" id="7"/>
-    <tableColumn name="Améliortions pour l'année prochaine" id="8"/>
-    <tableColumn name="Commentaires" id="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Enseignant"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Séance"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Groupe A1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Groupe A2-4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Groupe A3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Améliortions pour l'année prochaine"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Commentaires"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -339,10 +353,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -380,71 +394,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -472,7 +486,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -495,11 +509,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -508,13 +522,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -524,7 +538,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -533,7 +547,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -542,7 +556,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -550,10 +564,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -618,28 +632,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="7" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="41.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="46.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="79.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.453125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -668,7 +684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33">
+    <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45314</v>
       </c>
@@ -697,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33">
+    <row r="3" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>45315</v>
       </c>
@@ -720,7 +736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60.75">
+    <row r="4" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>45315</v>
       </c>
@@ -745,7 +761,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="74.25">
+    <row r="5" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>45315</v>
       </c>
@@ -770,7 +786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33">
+    <row r="6" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>45320</v>
       </c>
@@ -797,7 +813,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25">
+    <row r="7" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>45321</v>
       </c>
@@ -820,7 +836,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="60.75">
+    <row r="8" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>45321</v>
       </c>
@@ -843,7 +859,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="88.5">
+    <row r="9" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>45321</v>
       </c>
@@ -868,7 +884,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33">
+    <row r="10" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>45327</v>
       </c>
@@ -895,7 +911,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>45328</v>
       </c>
@@ -916,7 +932,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>45328</v>
       </c>
@@ -939,7 +955,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>45330</v>
       </c>
@@ -962,7 +978,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="51.75">
+    <row r="14" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>45335</v>
       </c>
@@ -985,7 +1001,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>45337</v>
       </c>
@@ -1008,7 +1024,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>45337</v>
       </c>
@@ -1033,7 +1049,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="50.25">
+    <row r="17" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>45349</v>
       </c>
@@ -1056,7 +1072,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="47.25">
+    <row r="18" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>45349</v>
       </c>
@@ -1079,7 +1095,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>45349</v>
       </c>
@@ -1104,7 +1120,7 @@
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="74.25">
+    <row r="20" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>45355</v>
       </c>
@@ -1127,7 +1143,7 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="74.25">
+    <row r="21" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>45355</v>
       </c>
@@ -1150,7 +1166,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="47.25">
+    <row r="22" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>45356</v>
       </c>
@@ -1171,7 +1187,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="47.25">
+    <row r="23" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>45362</v>
       </c>
@@ -1194,7 +1210,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="47.25">
+    <row r="24" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>45362</v>
       </c>
@@ -1217,7 +1233,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="39.75">
+    <row r="25" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>45362</v>
       </c>
@@ -1238,7 +1254,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row r="26" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>64</v>
       </c>
@@ -1259,29 +1275,53 @@
       <c r="H26" s="3"/>
       <c r="I26" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+    <row r="27" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <v>45370</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="I27" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <v>45370</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+      <c r="I28" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1292,7 +1332,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row r="30" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1303,7 +1343,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row r="31" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1314,7 +1354,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row r="32" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>

</xml_diff>